<commit_message>
updates for 2020 Baseball Season
</commit_message>
<xml_diff>
--- a/Laker fence sponsors.xlsx
+++ b/Laker fence sponsors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greg\Documents\Delavan Lakers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA24A90-3776-4CA2-8414-6B0526EB6DA2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E116D247-CFE0-4AB1-936D-164B32ABAE2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="93">
   <si>
     <t>Advanced Auto</t>
   </si>
@@ -150,18 +152,12 @@
     <t>Mulligan Insurance</t>
   </si>
   <si>
-    <t>LAKER SIGN SPONSORS 2019</t>
-  </si>
-  <si>
     <t>PHONE #</t>
   </si>
   <si>
     <t>CONTACT PERSON</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>262-749-9451</t>
   </si>
   <si>
@@ -174,9 +170,6 @@
     <t>262-548-8822 / 262-275-5771</t>
   </si>
   <si>
-    <t>728-6443</t>
-  </si>
-  <si>
     <t>262-745-4959</t>
   </si>
   <si>
@@ -201,12 +194,6 @@
     <t>Jaime Branton</t>
   </si>
   <si>
-    <t>Paid 2019</t>
-  </si>
-  <si>
-    <t>committed 2019</t>
-  </si>
-  <si>
     <t>262-728-2944</t>
   </si>
   <si>
@@ -229,9 +216,6 @@
   </si>
   <si>
     <t>Sign Needed</t>
-  </si>
-  <si>
-    <t>Paying</t>
   </si>
   <si>
     <t>Amount</t>
@@ -289,12 +273,6 @@
     <t>2020 Possibly</t>
   </si>
   <si>
-    <t>Paid</t>
-  </si>
-  <si>
-    <t>Credit</t>
-  </si>
-  <si>
     <t>checking with partners</t>
   </si>
   <si>
@@ -316,17 +294,39 @@
     <t>jamiebranton67@gmail.com</t>
   </si>
   <si>
-    <t>Sent in</t>
+    <t>watershedsaloon@yahoo.com</t>
+  </si>
+  <si>
+    <t>262-728-6443</t>
+  </si>
+  <si>
+    <t>theduckinn@att.net</t>
+  </si>
+  <si>
+    <t>purcellhunters@gmail.com</t>
+  </si>
+  <si>
+    <t>emilie@tntace.com</t>
+  </si>
+  <si>
+    <t>LAKER SIGN SPONSORS 2020</t>
+  </si>
+  <si>
+    <t>committed 2020</t>
+  </si>
+  <si>
+    <t>Paid 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,6 +373,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -395,12 +403,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -423,13 +431,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -445,7 +466,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -459,8 +479,16 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -759,34 +787,34 @@
     <col min="4" max="4" width="32.140625" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>67</v>
+      <c r="E1" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -799,17 +827,15 @@
       <c r="C2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="13" t="s">
+        <v>85</v>
+      </c>
       <c r="E2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="8">
-        <v>300</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -821,19 +847,15 @@
       <c r="C3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="13" t="s">
+        <v>87</v>
+      </c>
       <c r="E3" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H3" s="9">
-        <v>300</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -845,19 +867,15 @@
       <c r="C4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>76</v>
+      <c r="D4" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="8">
-        <v>300</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -867,21 +885,15 @@
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" s="9">
-        <v>300</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -895,41 +907,31 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="9">
-        <v>300</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>92</v>
+        <v>47</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>84</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="8">
-        <v>300</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -941,41 +943,35 @@
       <c r="C8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>87</v>
+      <c r="D8" s="13" t="s">
+        <v>79</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="8">
-        <v>300</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="8">
-        <v>300</v>
-      </c>
+      <c r="D9" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -985,19 +981,15 @@
         <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="8">
-        <v>300</v>
-      </c>
+      <c r="E10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -1010,18 +1002,12 @@
         <v>28</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11" s="8">
-        <v>0</v>
-      </c>
+      <c r="E11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -1035,17 +1021,11 @@
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" s="9">
-        <v>300</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="14"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -1055,21 +1035,15 @@
         <v>23</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H13" s="9">
-        <v>300</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -1079,131 +1053,115 @@
         <v>14</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="9">
-        <v>300</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>72</v>
+        <v>50</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H15" s="8">
-        <v>300</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="F16" s="3" t="s">
+      <c r="E17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="8">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="8"/>
+        <v>78</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="15"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>61</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="8"/>
+        <v>64</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="15"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
@@ -1211,37 +1169,37 @@
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="8"/>
+        <v>46</v>
+      </c>
+      <c r="G20" s="18"/>
+      <c r="H20" s="15"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="8"/>
+        <v>49</v>
+      </c>
+      <c r="G21" s="17"/>
+      <c r="H21" s="15"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
@@ -1249,55 +1207,55 @@
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="8"/>
+        <v>74</v>
+      </c>
+      <c r="G22" s="17"/>
+      <c r="H22" s="15"/>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="8"/>
+        <v>46</v>
+      </c>
+      <c r="G23" s="18"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="8"/>
+        <v>77</v>
+      </c>
+      <c r="G24" s="18"/>
+      <c r="H24" s="15"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
@@ -1306,42 +1264,47 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="5"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>69</v>
+      <c r="A26" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="8">
+      <c r="G26" s="8">
+        <f>SUM(G2:G25)</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="15">
         <f>SUM(H2:H25)</f>
-        <v>4200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>68</v>
+      <c r="A27" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
+      <c r="A28" s="9"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
+      <c r="A29" s="9"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
+      <c r="A30" s="9"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G25">
@@ -1354,9 +1317,13 @@
     <hyperlink ref="D9" r:id="rId4" xr:uid="{FB5615AF-BF49-4AD8-8B22-DA1BAE66FE03}"/>
     <hyperlink ref="D8" r:id="rId5" xr:uid="{D5D0DE07-9E81-4999-8039-F11B55AFF576}"/>
     <hyperlink ref="D7" r:id="rId6" xr:uid="{EAD87230-F769-4F5F-84AD-645AB4606997}"/>
+    <hyperlink ref="D2" r:id="rId7" xr:uid="{1BA902E9-FA66-4FCB-9172-F33B6B1D7773}"/>
+    <hyperlink ref="D3" r:id="rId8" xr:uid="{85363291-226A-4C67-AEDB-8AEEBE042AC7}"/>
+    <hyperlink ref="D16" r:id="rId9" display="mailto:purcellhunters@gmail.com" xr:uid="{36DC56F2-B4BE-4704-8192-C5E3155DF33A}"/>
+    <hyperlink ref="D17" r:id="rId10" xr:uid="{9D4C555F-8CA1-474C-A9EB-A72F378B151C}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0" right="0" top="0.5" bottom="0.5" header="0" footer="0"/>
-  <pageSetup scale="90" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId7"/>
+  <pageSetup scale="90" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>